<commit_message>
Update RFID circular antenna calculation
</commit_message>
<xml_diff>
--- a/Design_Guide/RFID_Antenna_calculator.xlsx
+++ b/Design_Guide/RFID_Antenna_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylvain Rouland\Desktop\PCB\Design_Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C27B7D4-D1F6-417C-8A5A-F70B03D4C152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE65228F-7338-4FAA-85C9-FBB3DA1ADFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6010" yWindow="0" windowWidth="18032" windowHeight="9341" xr2:uid="{7D0164FF-D231-499E-B11E-A128F9C4849E}"/>
+    <workbookView xWindow="-2918" yWindow="2317" windowWidth="7989" windowHeight="8690" xr2:uid="{7D0164FF-D231-499E-B11E-A128F9C4849E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>w</t>
   </si>
@@ -66,24 +66,12 @@
     <t>Nc</t>
   </si>
   <si>
-    <t>Davg</t>
-  </si>
-  <si>
-    <t>Average antenna diamter (cm)</t>
-  </si>
-  <si>
     <t>Equivalent diameter of track</t>
   </si>
   <si>
     <t>d</t>
   </si>
   <si>
-    <t>Average antenna circunference</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -157,12 +145,31 @@
   </si>
   <si>
     <t>13.56MHz</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Thickness of the winding</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Average antenna radius (cm)</t>
+  </si>
+  <si>
+    <t>Antenna inductance (H)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -479,11 +486,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,9 +515,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -554,6 +569,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,6 +585,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -585,58 +621,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>49834</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>397481</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>57237</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FE6A41-2328-4E6B-B78D-B7C244D9C1AC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3501694" y="45720"/>
-          <a:ext cx="2786047" cy="2435915"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>42478</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>27937</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>24435</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -653,7 +645,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -662,6 +654,94 @@
         <a:xfrm>
           <a:off x="3494338" y="3368040"/>
           <a:ext cx="3033459" cy="1973166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>119269</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>162901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>20746</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>26389</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53834CE-98FE-4809-A2B1-3A38566966D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3721210" y="7048731"/>
+          <a:ext cx="3718103" cy="1413992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>137796</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>546015</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>87120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93A57EAC-0185-4F97-9B23-850A7C123BB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4786685" y="8574130"/>
+          <a:ext cx="1269584" cy="1118166"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -970,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B0610D-8B17-48D9-9140-3610ED32B6C6}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -984,357 +1064,357 @@
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="14">
-        <f>C4-C8*(C7+C6)</f>
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5">
-        <f>(2*(C6+C7))/PI()</f>
-        <v>0.38197186342054879</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5">
-        <f>C10*PI()</f>
-        <v>35.185837720205683</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="C11" s="4">
         <v>1.75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="20">
-        <f>0.001*2*C12*(LN(C12/C11)-1.07)*C8^C13</f>
-        <v>1.661740499226545</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="4">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="8">
+    <row r="12" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7">
         <f>4*PI()*10^(-7)</f>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+    <row r="13" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13">
+        <f>(2*(C7+C8))/PI()</f>
+        <v>0.18398311421423102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4">
+        <f>C5-C10*(C8+C9)</f>
+        <v>117.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4">
+        <f>C6-C10*(C8+C9)</f>
+        <v>117.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4">
+        <f>C15*LN((2*C15*C16)/(C14*(C15+SQRT(C15*C15+C16*C16))))</f>
+        <v>736.56614061619553</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4">
+        <f>C16*LN((2*C15*C16)/(C14*(C16+SQRT(C15*C15+C16*C16))))</f>
+        <v>736.56614061619553</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4">
+        <f>2*(C15+C16-SQRT(C15*C15+C16*C16))</f>
+        <v>137.61294992731251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7">
+        <f>(C15+C16)/4</f>
+        <v>58.73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="19">
+        <f>10^(3)*(C12/PI())*(C17+C18-C19+C20)*C10^C11</f>
+        <v>9.3239072303013089</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="14">
-        <f>(2*(C21+C22))/PI()</f>
-        <v>0.34059157821665603</v>
+      <c r="A28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.254</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C29" s="4">
-        <f>C19-C24*(C22+C23)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="4">
-        <f>C20-C24*(C22+C23)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="4">
-        <f>C29*LN((2*C29*C30)/(C28*(C29+SQRT(C29*C29+C30*C30))))</f>
-        <v>102.69301639460471</v>
-      </c>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="4">
-        <f>C30*LN((2*C29*C30)/(C28*(C30+SQRT(C29*C29+C30*C30))))</f>
-        <v>102.69301639460471</v>
+      <c r="A32" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="22">
+        <f>(C26-C30/2*(C29+C28)/10)/200</f>
+        <v>1.9169000000000002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="30">
+        <f>C30*(C29+C28)/1000</f>
+        <v>3.3240000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="4">
-        <f>2*(C29+C30-SQRT(C29*C29+C30*C30))</f>
-        <v>29.289321881345245</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="8">
-        <f>(C29+C30)/4</f>
-        <v>12.5</v>
+      <c r="B34" s="2"/>
+      <c r="C34" s="30">
+        <f>4*PI()*10^(-7)</f>
+        <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="31"/>
     </row>
     <row r="36" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="20">
-        <f>10^(3)*(C26/PI())*(C31+C32-C33+C34)*C24^C25</f>
-        <v>1.2612222197007521</v>
+      <c r="A36" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="29">
+        <f>31.33*C34*C30*C30*(C32*C32)/(8*C32+11*C33)</f>
+        <v>2.7422694143104424E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="32">
+        <f>C36*1000000</f>
+        <v>2.7422694143104422</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1342,21 +1422,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045B459AFED191C4AAE8845CA3F3FDE0C" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0659c2525336b15891f44f465e776bd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5e56b44-5447-4865-8f3e-d434c1f11eec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e10b04a967fcd5b345ab7a4b7dbfb242" ns2:_="">
     <xsd:import namespace="b5e56b44-5447-4865-8f3e-d434c1f11eec"/>
@@ -1526,24 +1591,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05CF64F-B391-481E-8C3E-26AAADF831E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{488B49BD-4804-4BCD-9C52-BA8FF9FD856D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E81F3F4-A374-4257-B050-35BE60331892}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1559,4 +1622,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{488B49BD-4804-4BCD-9C52-BA8FF9FD856D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05CF64F-B391-481E-8C3E-26AAADF831E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>